<commit_message>
Fixed issue with dispatch model
</commit_message>
<xml_diff>
--- a/inputs/PGE_Resources.xlsx
+++ b/inputs/PGE_Resources.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4460" yWindow="0" windowWidth="24160" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="90">
   <si>
     <t>In-service date</t>
   </si>
@@ -84,190 +85,211 @@
     <t>Jan Capacity (MW)</t>
   </si>
   <si>
+    <t>Biglow Canyon I</t>
+  </si>
+  <si>
+    <t>Biglow Canyon II</t>
+  </si>
+  <si>
+    <t>Biglow Canyon III</t>
+  </si>
+  <si>
+    <t>Tucannon</t>
+  </si>
+  <si>
+    <t>Oak Grove</t>
+  </si>
+  <si>
+    <t>North Fork</t>
+  </si>
+  <si>
+    <t>Faraday</t>
+  </si>
+  <si>
+    <t>River Mill</t>
+  </si>
+  <si>
+    <t>Sullivan</t>
+  </si>
+  <si>
+    <t>Round Butte</t>
+  </si>
+  <si>
+    <t>Pelton</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Hydro</t>
+  </si>
+  <si>
+    <t>Energy Potential (Mwa)</t>
+  </si>
+  <si>
+    <t>Wells</t>
+  </si>
+  <si>
+    <t>Grant PUD Deal</t>
+  </si>
+  <si>
+    <t>Canadian Entitlement Extension</t>
+  </si>
+  <si>
+    <t>PPM Klondike II</t>
+  </si>
+  <si>
+    <t>Vansycle Ridge</t>
+  </si>
+  <si>
+    <t>Small QF Contracts</t>
+  </si>
+  <si>
+    <t>QF</t>
+  </si>
+  <si>
+    <t>Small Renewable Contracts</t>
+  </si>
+  <si>
+    <t>Renewable</t>
+  </si>
+  <si>
+    <t>Dispatchable Standby Generation</t>
+  </si>
+  <si>
+    <t>Demand Response</t>
+  </si>
+  <si>
+    <t>Bi-Seasonal Capacity</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>93MW available 2013</t>
+  </si>
+  <si>
+    <t>Plus 20MW of duct firing; HR = 6,800 Btu/kWh</t>
+  </si>
+  <si>
+    <t>HR = 9,260 Btu/kWh</t>
+  </si>
+  <si>
+    <t>HR = 7,100 Btu/kWh</t>
+  </si>
+  <si>
+    <t>CF = 31.8%</t>
+  </si>
+  <si>
+    <t>Total capacity = 450MW</t>
+  </si>
+  <si>
+    <t>Reservoir storage capability; Expires 2055</t>
+  </si>
+  <si>
+    <t>Willamette Falls; Expires 2035</t>
+  </si>
+  <si>
+    <t>Clackamas River; Expires 2055</t>
+  </si>
+  <si>
+    <t>PPA expires 2027</t>
+  </si>
+  <si>
+    <t>Contracted with Douglas County PUD</t>
+  </si>
+  <si>
+    <t>In 2022, the Tribes gain another 1/6 share of the plant, reducing ownership to slightly more than 50%</t>
+  </si>
+  <si>
+    <t>Iberdrola Renewables Seasonal Capacity Contract</t>
+  </si>
+  <si>
+    <t>PaTu Wind</t>
+  </si>
+  <si>
+    <t>Coffin Butte expires 2027 (5.7MW); Green Lane Energy expires 2022 (1.6MW)</t>
+  </si>
+  <si>
+    <t>Small Scale Solar</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Eugene Water and Electric Board expires middle of 2014</t>
+  </si>
+  <si>
+    <t>Spokane Energy (formerly Washington Water Power) extends through 2017</t>
+  </si>
+  <si>
+    <t>Expires mid 2016</t>
+  </si>
+  <si>
+    <t>26797_Onshore</t>
+  </si>
+  <si>
+    <t>23095_Offshore</t>
+  </si>
+  <si>
+    <t>Our IRP Expansion</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Portland_PV</t>
+  </si>
+  <si>
+    <t>Burns_PV</t>
+  </si>
+  <si>
+    <t>Rated Capacity (MW)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Var O&amp;M ($/MWh)</t>
+  </si>
+  <si>
+    <t>Heatrate (btu/kWh)</t>
+  </si>
+  <si>
+    <t>HR from an Oregon State study</t>
+  </si>
+  <si>
+    <t>Colstrip, Montana; HR from AVISTA</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M ($/kW)</t>
+  </si>
+  <si>
+    <t>2003 contract extended to 2024. $3mil per year</t>
+  </si>
+  <si>
+    <t>ALL HYDRO PRICES FROM E3 STUDY!</t>
+  </si>
+  <si>
+    <t>Flat Rate</t>
+  </si>
+  <si>
+    <t>On Peak</t>
+  </si>
+  <si>
+    <t>Off Peak</t>
+  </si>
+  <si>
+    <t>Levelized cost of energy ($/MWh)</t>
+  </si>
+  <si>
+    <t>March 2014 spot price (Northwest)</t>
+  </si>
+  <si>
     <t>Coal</t>
   </si>
   <si>
     <t>Gas</t>
-  </si>
-  <si>
-    <t>Biglow Canyon I</t>
-  </si>
-  <si>
-    <t>Biglow Canyon II</t>
-  </si>
-  <si>
-    <t>Biglow Canyon III</t>
-  </si>
-  <si>
-    <t>Tucannon</t>
-  </si>
-  <si>
-    <t>Oak Grove</t>
-  </si>
-  <si>
-    <t>North Fork</t>
-  </si>
-  <si>
-    <t>Faraday</t>
-  </si>
-  <si>
-    <t>River Mill</t>
-  </si>
-  <si>
-    <t>Sullivan</t>
-  </si>
-  <si>
-    <t>Round Butte</t>
-  </si>
-  <si>
-    <t>Pelton</t>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Hydro</t>
-  </si>
-  <si>
-    <t>Energy Potential (Mwa)</t>
-  </si>
-  <si>
-    <t>Wells</t>
-  </si>
-  <si>
-    <t>Grant PUD Deal</t>
-  </si>
-  <si>
-    <t>Canadian Entitlement Extension</t>
-  </si>
-  <si>
-    <t>PPM Klondike II</t>
-  </si>
-  <si>
-    <t>Vansycle Ridge</t>
-  </si>
-  <si>
-    <t>Small QF Contracts</t>
-  </si>
-  <si>
-    <t>QF</t>
-  </si>
-  <si>
-    <t>Small Renewable Contracts</t>
-  </si>
-  <si>
-    <t>Renewable</t>
-  </si>
-  <si>
-    <t>Dispatchable Standby Generation</t>
-  </si>
-  <si>
-    <t>Demand Response</t>
-  </si>
-  <si>
-    <t>Bi-Seasonal Capacity</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>93MW available 2013</t>
-  </si>
-  <si>
-    <t>Plus 20MW of duct firing; HR = 6,800 Btu/kWh</t>
-  </si>
-  <si>
-    <t>HR = 9,260 Btu/kWh</t>
-  </si>
-  <si>
-    <t>HR = 7,100 Btu/kWh</t>
-  </si>
-  <si>
-    <t>Colstrip, Montana</t>
-  </si>
-  <si>
-    <t>CF = 31.8%</t>
-  </si>
-  <si>
-    <t>Total capacity = 450MW</t>
-  </si>
-  <si>
-    <t>Reservoir storage capability; Expires 2055</t>
-  </si>
-  <si>
-    <t>Willamette Falls; Expires 2035</t>
-  </si>
-  <si>
-    <t>Clackamas River; Expires 2055</t>
-  </si>
-  <si>
-    <t>PPA expires 2027</t>
-  </si>
-  <si>
-    <t>Contracted with Douglas County PUD</t>
-  </si>
-  <si>
-    <t>In 2022, the Tribes gain another 1/6 share of the plant, reducing ownership to slightly more than 50%</t>
-  </si>
-  <si>
-    <t>2003 contract extended to 2024</t>
-  </si>
-  <si>
-    <t>Iberdrola Renewables Seasonal Capacity Contract</t>
-  </si>
-  <si>
-    <t>PaTu Wind</t>
-  </si>
-  <si>
-    <t>Coffin Butte expires 2027 (5.7MW); Green Lane Energy expires 2022 (1.6MW)</t>
-  </si>
-  <si>
-    <t>Small Scale Solar</t>
-  </si>
-  <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>Eugene Water and Electric Board expires middle of 2014</t>
-  </si>
-  <si>
-    <t>Spokane Energy (formerly Washington Water Power) extends through 2017</t>
-  </si>
-  <si>
-    <t>Expires mid 2016</t>
-  </si>
-  <si>
-    <t>26797_Onshore</t>
-  </si>
-  <si>
-    <t>23095_Offshore</t>
-  </si>
-  <si>
-    <t>Our IRP Expansion</t>
-  </si>
-  <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>Portland_PV</t>
-  </si>
-  <si>
-    <t>Burns_PV</t>
-  </si>
-  <si>
-    <t>Rated Capacity (MW)</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Var O&amp;M ($/MWh)</t>
-  </si>
-  <si>
-    <t>Heatrate (btu/kWh)</t>
-  </si>
-  <si>
-    <t>Fixed O&amp;M ($/kW)</t>
   </si>
 </sst>
 </file>
@@ -316,8 +338,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -420,7 +484,7 @@
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -467,6 +531,27 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -513,6 +598,27 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -845,34 +951,35 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="43.83203125" customWidth="1"/>
+    <col min="8" max="8" width="43.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="65" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -881,24 +988,24 @@
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>80</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>75</v>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C2">
         <v>58</v>
@@ -917,8 +1024,8 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>35</v>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C3">
         <v>36</v>
@@ -931,14 +1038,23 @@
       </c>
       <c r="G3">
         <v>2017</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J3">
+        <v>3.55</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>75</v>
+      <c r="B4" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -957,8 +1073,8 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>75</v>
+      <c r="B5" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -972,16 +1088,16 @@
       <c r="G5">
         <v>2016</v>
       </c>
-      <c r="H5" t="s">
-        <v>71</v>
+      <c r="H5" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>75</v>
+      <c r="B6" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C6">
         <v>167</v>
@@ -995,16 +1111,16 @@
       <c r="G6">
         <v>2014</v>
       </c>
-      <c r="H6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="H6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>75</v>
+      <c r="B7" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C7">
         <v>150</v>
@@ -1018,16 +1134,16 @@
       <c r="G7">
         <v>2016</v>
       </c>
-      <c r="H7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="H7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>75</v>
+      <c r="B8" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -1041,16 +1157,16 @@
       <c r="G8">
         <v>2014</v>
       </c>
-      <c r="H8" t="s">
-        <v>69</v>
+      <c r="H8" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
+      <c r="B9" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C9">
         <v>374</v>
@@ -1066,14 +1182,26 @@
       </c>
       <c r="G9">
         <v>9999</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="1">
+        <v>23.44</v>
+      </c>
+      <c r="J9">
+        <v>3.78</v>
+      </c>
+      <c r="K9">
+        <v>9911</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
+      <c r="B10" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="C10">
         <v>296</v>
@@ -1090,22 +1218,28 @@
       <c r="G10">
         <v>9999</v>
       </c>
-      <c r="H10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
+      <c r="H10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="1">
+        <v>23.44</v>
+      </c>
+      <c r="J10">
+        <v>3.78</v>
+      </c>
+      <c r="K10">
+        <v>11950</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>22</v>
+      <c r="B11" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C11">
-        <v>3050</v>
+        <v>346</v>
       </c>
       <c r="D11">
         <v>346</v>
@@ -1119,25 +1253,25 @@
       <c r="G11">
         <v>9999</v>
       </c>
-      <c r="H11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
+      <c r="H11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="1">
+        <v>10.28</v>
       </c>
       <c r="J11">
+        <v>3.23</v>
+      </c>
+      <c r="K11">
         <v>9260</v>
-      </c>
-      <c r="K11">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>22</v>
+      <c r="B12" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C12">
         <v>163</v>
@@ -1154,16 +1288,22 @@
       <c r="G12">
         <v>9999</v>
       </c>
-      <c r="I12">
-        <v>3</v>
+      <c r="I12" s="1">
+        <v>10.28</v>
+      </c>
+      <c r="J12">
+        <v>3.23</v>
+      </c>
+      <c r="K12">
+        <v>9260</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>22</v>
+      <c r="B13" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C13">
         <v>21</v>
@@ -1180,16 +1320,22 @@
       <c r="G13">
         <v>9999</v>
       </c>
-      <c r="I13">
-        <v>3</v>
+      <c r="I13" s="1">
+        <v>10.28</v>
+      </c>
+      <c r="J13">
+        <v>3.23</v>
+      </c>
+      <c r="K13">
+        <v>9260</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
+      <c r="B14" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C14">
         <v>222</v>
@@ -1206,16 +1352,22 @@
       <c r="G14">
         <v>9999</v>
       </c>
-      <c r="I14">
-        <v>4</v>
+      <c r="I14" s="1">
+        <v>10.28</v>
+      </c>
+      <c r="J14">
+        <v>3.23</v>
+      </c>
+      <c r="K14">
+        <v>6800</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
+      <c r="B15" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C15">
         <v>394</v>
@@ -1232,25 +1384,25 @@
       <c r="G15">
         <v>9999</v>
       </c>
-      <c r="H15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15">
-        <v>4</v>
+      <c r="H15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="1">
+        <v>10.28</v>
       </c>
       <c r="J15">
+        <v>3.23</v>
+      </c>
+      <c r="K15">
         <v>6800</v>
-      </c>
-      <c r="K15">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
+      <c r="B16" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C16">
         <v>260</v>
@@ -1267,25 +1419,25 @@
       <c r="G16">
         <v>9999</v>
       </c>
-      <c r="H16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16">
-        <v>4</v>
+      <c r="H16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="1">
+        <v>10.28</v>
       </c>
       <c r="J16">
+        <v>3.23</v>
+      </c>
+      <c r="K16">
         <v>7100</v>
       </c>
-      <c r="K16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
-        <v>22</v>
+      <c r="B17" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C17">
         <v>441</v>
@@ -1302,19 +1454,26 @@
       <c r="G17">
         <v>9999</v>
       </c>
-      <c r="I17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="1">
+        <v>10.28</v>
+      </c>
+      <c r="J17">
+        <v>3.23</v>
+      </c>
+      <c r="K17">
+        <v>7043</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <f>450/3</f>
+        <v>150</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -1328,22 +1487,26 @@
       <c r="G18">
         <v>9999</v>
       </c>
-      <c r="H18" t="s">
-        <v>55</v>
-      </c>
-      <c r="I18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="H18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J18">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <f t="shared" ref="C19:C20" si="0">450/3</f>
+        <v>150</v>
       </c>
       <c r="D19">
         <v>8</v>
@@ -1357,22 +1520,26 @@
       <c r="G19">
         <v>9999</v>
       </c>
-      <c r="H19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="H19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J19">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
       <c r="D20">
         <v>8</v>
@@ -1386,19 +1553,22 @@
       <c r="G20">
         <v>9999</v>
       </c>
-      <c r="I20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="I20" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J20">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>13</v>
+        <v>267</v>
       </c>
       <c r="D21">
         <v>13</v>
@@ -1412,18 +1582,18 @@
       <c r="G21">
         <v>9999</v>
       </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I21" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J21">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D22">
@@ -1438,22 +1608,22 @@
       <c r="G22">
         <v>2055</v>
       </c>
-      <c r="H22" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="H22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J22">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D23">
         <v>43</v>
@@ -1467,22 +1637,22 @@
       <c r="G23">
         <v>2055</v>
       </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-      <c r="I23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="H23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J23">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D24">
         <v>43</v>
@@ -1496,19 +1666,22 @@
       <c r="G24">
         <v>2055</v>
       </c>
-      <c r="H24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="H24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J24">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D25">
         <v>23</v>
@@ -1522,19 +1695,22 @@
       <c r="G25">
         <v>2055</v>
       </c>
-      <c r="H25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="H25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J25">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26">
-        <v>16</v>
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D26">
         <v>16</v>
@@ -1548,19 +1724,22 @@
       <c r="G26">
         <v>2035</v>
       </c>
-      <c r="H26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="H26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J26">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27">
-        <v>225</v>
+        <v>30</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D27">
         <v>225</v>
@@ -1574,19 +1753,22 @@
       <c r="G27">
         <v>2055</v>
       </c>
-      <c r="H27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="H27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J27">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28">
-        <v>73</v>
       </c>
       <c r="D28">
         <v>73</v>
@@ -1600,19 +1782,22 @@
       <c r="G28">
         <v>2055</v>
       </c>
-      <c r="H28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="H28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J28">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="C29">
-        <v>147</v>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D29">
         <v>147</v>
@@ -1626,19 +1811,22 @@
       <c r="G29">
         <v>2018</v>
       </c>
-      <c r="H29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="H29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I29" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J29">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30">
-        <v>143</v>
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D30">
         <v>143</v>
@@ -1652,16 +1840,19 @@
       <c r="G30">
         <v>2052</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="I30" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J30">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31">
-        <v>36</v>
+      <c r="B31" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D31">
         <v>36</v>
@@ -1675,16 +1866,19 @@
       <c r="G31">
         <v>9999</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="30">
+      <c r="I31" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J31">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30">
       <c r="A32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D32">
         <v>-20</v>
@@ -1698,16 +1892,22 @@
       <c r="G32">
         <v>2024</v>
       </c>
-      <c r="H32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="H32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="J32">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C33">
         <v>75</v>
@@ -1724,13 +1924,19 @@
       <c r="G33">
         <v>9999</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J33">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C34">
         <v>25</v>
@@ -1747,19 +1953,22 @@
       <c r="G34">
         <v>2027</v>
       </c>
-      <c r="H34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="H34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J34">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30">
       <c r="A35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
+        <v>40</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D35">
         <v>7</v>
@@ -1773,19 +1982,16 @@
       <c r="G35">
         <v>9999</v>
       </c>
-      <c r="H35" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="H35" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1799,16 +2005,19 @@
       <c r="G36">
         <v>9999</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="30">
+      <c r="I36" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J36">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30">
       <c r="A37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
       </c>
       <c r="D37">
         <v>116</v>
@@ -1822,19 +2031,16 @@
       <c r="G37">
         <v>9999</v>
       </c>
-      <c r="H37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="H37" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C38">
-        <v>5</v>
       </c>
       <c r="D38">
         <v>45</v>
@@ -1849,15 +2055,12 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
       </c>
       <c r="D39">
         <v>100</v>
@@ -1871,16 +2074,16 @@
       <c r="G39">
         <v>2019</v>
       </c>
-      <c r="H39" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="H39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" t="s">
-        <v>34</v>
+        <v>61</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C40">
         <v>9</v>
@@ -1891,13 +2094,19 @@
       <c r="G40">
         <v>2030</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J40">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C41">
         <v>13</v>
@@ -1905,13 +2114,19 @@
       <c r="E41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" s="1">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="J41">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" t="s">
-        <v>34</v>
+        <v>68</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -1922,16 +2137,22 @@
       <c r="G42">
         <v>2035</v>
       </c>
-      <c r="H42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="H42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I42" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J42">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" t="s">
-        <v>34</v>
+        <v>69</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C43">
         <v>10</v>
@@ -1942,19 +2163,25 @@
       <c r="G43">
         <v>2035</v>
       </c>
-      <c r="H43" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="H43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I43" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="J43">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C44">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F44">
         <v>2014</v>
@@ -1962,16 +2189,22 @@
       <c r="G44">
         <v>2035</v>
       </c>
-      <c r="H44" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="H44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I44" s="1">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="J44">
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -1982,8 +2215,84 @@
       <c r="G45">
         <v>2035</v>
       </c>
-      <c r="H45" t="s">
-        <v>74</v>
+      <c r="H45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I45" s="1">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="J45">
+        <v>2.87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2">
+        <v>43.22</v>
+      </c>
+      <c r="C2">
+        <v>43.22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>49.27</v>
+      </c>
+      <c r="C3">
+        <v>49.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4">
+        <v>35.159999999999997</v>
+      </c>
+      <c r="C4">
+        <v>35.159999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6">
+        <v>30.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added hydro to dispatch
</commit_message>
<xml_diff>
--- a/inputs/PGE_Resources.xlsx
+++ b/inputs/PGE_Resources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="0" windowWidth="24160" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
   <si>
     <t>In-service date</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Carty</t>
   </si>
   <si>
-    <t>Jan Capacity (MW)</t>
-  </si>
-  <si>
     <t>Biglow Canyon I</t>
   </si>
   <si>
@@ -121,21 +118,12 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>Hydro</t>
-  </si>
-  <si>
-    <t>Energy Potential (Mwa)</t>
-  </si>
-  <si>
     <t>Wells</t>
   </si>
   <si>
     <t>Grant PUD Deal</t>
   </si>
   <si>
-    <t>Canadian Entitlement Extension</t>
-  </si>
-  <si>
     <t>PPM Klondike II</t>
   </si>
   <si>
@@ -151,9 +139,6 @@
     <t>Small Renewable Contracts</t>
   </si>
   <si>
-    <t>Renewable</t>
-  </si>
-  <si>
     <t>Dispatchable Standby Generation</t>
   </si>
   <si>
@@ -265,9 +250,6 @@
     <t>Fixed O&amp;M ($/kW)</t>
   </si>
   <si>
-    <t>2003 contract extended to 2024. $3mil per year</t>
-  </si>
-  <si>
     <t>ALL HYDRO PRICES FROM E3 STUDY!</t>
   </si>
   <si>
@@ -290,6 +272,18 @@
   </si>
   <si>
     <t>Gas</t>
+  </si>
+  <si>
+    <t>Energy Potential (MWh/year)</t>
+  </si>
+  <si>
+    <t>Reservoir</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>STUPID</t>
   </si>
 </sst>
 </file>
@@ -338,8 +332,86 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -484,7 +556,7 @@
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -552,6 +624,45 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -619,6 +730,45 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -948,1280 +1098,1259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
-    <col min="3" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="43.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="43.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="65" customHeight="1">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="65" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C2">
         <v>58</v>
       </c>
+      <c r="D2">
+        <v>262800</v>
+      </c>
       <c r="E2">
-        <v>30</v>
+        <v>2011</v>
       </c>
       <c r="F2">
-        <v>2011</v>
-      </c>
-      <c r="G2">
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>36</v>
       </c>
+      <c r="D3">
+        <v>87600</v>
+      </c>
       <c r="E3">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="F3">
-        <v>999</v>
-      </c>
-      <c r="G3">
         <v>2017</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="G3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="1">
         <v>14.15</v>
       </c>
-      <c r="J3">
+      <c r="I3">
         <v>3.55</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:10" ht="30">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C4">
         <v>16</v>
       </c>
+      <c r="D4">
+        <v>87600</v>
+      </c>
       <c r="E4">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="F4">
-        <v>999</v>
-      </c>
-      <c r="G4">
         <v>2014</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
+      <c r="D5">
+        <v>814680</v>
+      </c>
       <c r="E5">
-        <v>93</v>
+        <v>2006</v>
       </c>
       <c r="F5">
-        <v>2006</v>
-      </c>
-      <c r="G5">
         <v>2016</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="30">
+      <c r="G5" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C6">
         <v>167</v>
       </c>
+      <c r="D6">
+        <v>569400</v>
+      </c>
       <c r="E6">
-        <v>65</v>
+        <v>2011</v>
       </c>
       <c r="F6">
-        <v>2011</v>
-      </c>
-      <c r="G6">
         <v>2014</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30">
+      <c r="G6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>150</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="F7">
-        <v>999</v>
-      </c>
-      <c r="G7">
         <v>2016</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="30">
+      <c r="G7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="F8">
-        <v>999</v>
-      </c>
-      <c r="G8">
         <v>2014</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="G8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>374</v>
       </c>
       <c r="D9">
-        <v>374</v>
+        <v>2724360</v>
       </c>
       <c r="E9">
-        <v>311</v>
+        <v>1980</v>
       </c>
       <c r="F9">
-        <v>1980</v>
-      </c>
-      <c r="G9">
         <v>9999</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="G9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="1">
         <v>23.44</v>
       </c>
+      <c r="I9">
+        <v>3.78</v>
+      </c>
       <c r="J9">
-        <v>3.78</v>
-      </c>
-      <c r="K9">
         <v>9911</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C10">
         <v>296</v>
       </c>
       <c r="D10">
-        <v>296</v>
+        <v>2242560</v>
       </c>
       <c r="E10">
-        <v>256</v>
+        <v>1985</v>
       </c>
       <c r="F10">
-        <v>1985</v>
-      </c>
-      <c r="G10">
         <v>9999</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="1">
         <v>23.44</v>
       </c>
+      <c r="I10">
+        <v>3.78</v>
+      </c>
       <c r="J10">
-        <v>3.78</v>
-      </c>
-      <c r="K10">
         <v>11950</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C11">
         <v>346</v>
       </c>
       <c r="D11">
-        <v>346</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1976</v>
       </c>
       <c r="F11">
-        <v>1976</v>
-      </c>
-      <c r="G11">
         <v>9999</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="G11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="1">
         <v>10.28</v>
       </c>
+      <c r="I11">
+        <v>3.23</v>
+      </c>
       <c r="J11">
-        <v>3.23</v>
-      </c>
-      <c r="K11">
         <v>9260</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <v>163</v>
       </c>
       <c r="D12">
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1976</v>
       </c>
       <c r="F12">
-        <v>1976</v>
-      </c>
-      <c r="G12">
         <v>9999</v>
       </c>
-      <c r="I12" s="1">
+      <c r="H12" s="1">
         <v>10.28</v>
       </c>
+      <c r="I12">
+        <v>3.23</v>
+      </c>
       <c r="J12">
-        <v>3.23</v>
-      </c>
-      <c r="K12">
         <v>9260</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C13">
         <v>21</v>
       </c>
       <c r="D13">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1976</v>
       </c>
       <c r="F13">
-        <v>1976</v>
-      </c>
-      <c r="G13">
         <v>9999</v>
       </c>
-      <c r="I13" s="1">
+      <c r="H13" s="1">
         <v>10.28</v>
       </c>
+      <c r="I13">
+        <v>3.23</v>
+      </c>
       <c r="J13">
-        <v>3.23</v>
-      </c>
-      <c r="K13">
         <v>9260</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C14">
         <v>222</v>
       </c>
       <c r="D14">
-        <v>222</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>2015</v>
       </c>
       <c r="F14">
-        <v>2015</v>
-      </c>
-      <c r="G14">
         <v>9999</v>
       </c>
-      <c r="I14" s="1">
+      <c r="H14" s="1">
         <v>10.28</v>
       </c>
+      <c r="I14">
+        <v>3.23</v>
+      </c>
       <c r="J14">
-        <v>3.23</v>
-      </c>
-      <c r="K14">
         <v>6800</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C15">
         <v>394</v>
       </c>
       <c r="D15">
-        <v>394</v>
+        <v>3057240</v>
       </c>
       <c r="E15">
-        <v>349</v>
+        <v>2007</v>
       </c>
       <c r="F15">
-        <v>2007</v>
-      </c>
-      <c r="G15">
         <v>9999</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="G15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="1">
         <v>10.28</v>
       </c>
+      <c r="I15">
+        <v>3.23</v>
+      </c>
       <c r="J15">
-        <v>3.23</v>
-      </c>
-      <c r="K15">
         <v>6800</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C16">
         <v>260</v>
       </c>
       <c r="D16">
-        <v>260</v>
+        <v>2032320</v>
       </c>
       <c r="E16">
-        <v>232</v>
+        <v>1995</v>
       </c>
       <c r="F16">
-        <v>1995</v>
-      </c>
-      <c r="G16">
         <v>9999</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="G16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="1">
         <v>10.28</v>
       </c>
+      <c r="I16">
+        <v>3.23</v>
+      </c>
       <c r="J16">
-        <v>3.23</v>
-      </c>
-      <c r="K16">
         <v>7100</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <v>441</v>
       </c>
       <c r="D17">
-        <v>441</v>
+        <v>3188640</v>
       </c>
       <c r="E17">
-        <v>364</v>
+        <v>2016</v>
       </c>
       <c r="F17">
-        <v>2016</v>
-      </c>
-      <c r="G17">
         <v>9999</v>
       </c>
-      <c r="I17" s="1">
+      <c r="H17" s="1">
         <v>10.28</v>
       </c>
+      <c r="I17">
+        <v>3.23</v>
+      </c>
       <c r="J17">
-        <v>3.23</v>
-      </c>
-      <c r="K17">
         <v>7043</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <f>450/3</f>
         <v>150</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>350400</v>
       </c>
       <c r="E18">
-        <v>40</v>
+        <v>2008</v>
       </c>
       <c r="F18">
-        <v>2008</v>
-      </c>
-      <c r="G18">
         <v>9999</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="G18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J18">
+      <c r="I18">
         <v>3.63</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <f t="shared" ref="C19:C20" si="0">450/3</f>
         <v>150</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>481800</v>
       </c>
       <c r="E19">
-        <v>55</v>
+        <v>2010</v>
       </c>
       <c r="F19">
-        <v>2010</v>
-      </c>
-      <c r="G19">
         <v>9999</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="G19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J19">
+      <c r="I19">
         <v>3.63</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>429240</v>
       </c>
       <c r="E20">
-        <v>49</v>
+        <v>2011</v>
       </c>
       <c r="F20">
-        <v>2011</v>
-      </c>
-      <c r="G20">
         <v>9999</v>
       </c>
-      <c r="I20" s="1">
+      <c r="H20" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J20">
+      <c r="I20">
         <v>3.63</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>267</v>
       </c>
       <c r="D21">
-        <v>13</v>
+        <v>893520</v>
       </c>
       <c r="E21">
-        <v>102</v>
+        <v>2015</v>
       </c>
       <c r="F21">
-        <v>2015</v>
-      </c>
-      <c r="G21">
         <v>9999</v>
       </c>
-      <c r="I21" s="1">
+      <c r="H21" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J21">
+      <c r="I21">
         <v>3.63</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>201480</v>
+      </c>
+      <c r="E22">
+        <v>1924</v>
+      </c>
+      <c r="F22">
+        <v>2055</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I22">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23">
+        <v>43</v>
+      </c>
+      <c r="D23">
+        <v>201480</v>
+      </c>
+      <c r="E23">
+        <v>1958</v>
+      </c>
+      <c r="F23">
+        <v>2055</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I23">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>166440</v>
+      </c>
+      <c r="E24">
+        <v>1907</v>
+      </c>
+      <c r="F24">
+        <v>2055</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I24">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>105120</v>
+      </c>
+      <c r="E25">
+        <v>1911</v>
+      </c>
+      <c r="F25">
+        <v>2055</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I25">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>122640</v>
+      </c>
+      <c r="E26">
+        <v>1895</v>
+      </c>
+      <c r="F26">
+        <v>2035</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I26">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27">
+        <v>298</v>
+      </c>
+      <c r="D27">
+        <f>110*8760</f>
+        <v>963600</v>
+      </c>
+      <c r="E27">
+        <v>1964</v>
+      </c>
+      <c r="F27">
+        <v>2055</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I27">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28">
+        <v>225</v>
+      </c>
+      <c r="D28">
+        <v>674520</v>
+      </c>
+      <c r="E28">
+        <v>1964</v>
+      </c>
+      <c r="F28">
+        <v>2055</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I28">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29">
+        <v>73</v>
+      </c>
+      <c r="D29">
+        <v>297840</v>
+      </c>
+      <c r="E29">
+        <v>1957</v>
+      </c>
+      <c r="F29">
+        <v>2055</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I29">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30">
+        <v>147</v>
+      </c>
+      <c r="D30">
+        <v>884760</v>
+      </c>
+      <c r="E30">
+        <v>999</v>
+      </c>
+      <c r="F30">
+        <v>2018</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" s="1">
+        <v>14.15</v>
+      </c>
+      <c r="I30">
+        <v>3.55</v>
+      </c>
+      <c r="J30">
+        <f>SUM(D28:D29)/8760</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D22">
-        <v>33</v>
-      </c>
-      <c r="E22">
-        <v>23</v>
-      </c>
-      <c r="F22">
-        <v>1924</v>
-      </c>
-      <c r="G22">
-        <v>2055</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31">
+        <v>123</v>
+      </c>
+      <c r="D31">
+        <f>762120-87600</f>
+        <v>674520</v>
+      </c>
+      <c r="E31">
+        <v>999</v>
+      </c>
+      <c r="F31">
+        <v>2052</v>
+      </c>
+      <c r="H31" s="1">
         <v>14.15</v>
       </c>
-      <c r="J22">
+      <c r="I31">
         <v>3.55</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23">
-        <v>43</v>
-      </c>
-      <c r="E23">
-        <v>23</v>
-      </c>
-      <c r="F23">
-        <v>1958</v>
-      </c>
-      <c r="G23">
-        <v>2055</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="1">
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>61320</v>
+      </c>
+      <c r="E32">
+        <v>999</v>
+      </c>
+      <c r="F32">
+        <v>9999</v>
+      </c>
+      <c r="H32" s="1">
         <v>14.15</v>
       </c>
-      <c r="J23">
+      <c r="I32">
         <v>3.55</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24">
-        <v>43</v>
-      </c>
-      <c r="E24">
-        <v>19</v>
-      </c>
-      <c r="F24">
-        <v>1907</v>
-      </c>
-      <c r="G24">
-        <v>2055</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J24">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25">
-        <v>23</v>
-      </c>
-      <c r="E25">
-        <v>12</v>
-      </c>
-      <c r="F25">
-        <v>1911</v>
-      </c>
-      <c r="G25">
-        <v>2055</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J25">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26">
-        <v>16</v>
-      </c>
-      <c r="E26">
-        <v>14</v>
-      </c>
-      <c r="F26">
-        <v>1895</v>
-      </c>
-      <c r="G26">
-        <v>2035</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I26" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J26">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27">
-        <v>225</v>
-      </c>
-      <c r="E27">
-        <v>77</v>
-      </c>
-      <c r="F27">
-        <v>1964</v>
-      </c>
-      <c r="G27">
-        <v>2055</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J27">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="1" t="s">
+    <row r="33" spans="1:9">
+      <c r="A33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28">
-        <v>73</v>
-      </c>
-      <c r="E28">
-        <v>34</v>
-      </c>
-      <c r="F28">
-        <v>1957</v>
-      </c>
-      <c r="G28">
-        <v>2055</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I28" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J28">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29">
-        <v>147</v>
-      </c>
-      <c r="E29">
-        <v>101</v>
-      </c>
-      <c r="F29">
-        <v>999</v>
-      </c>
-      <c r="G29">
-        <v>2018</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I29" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J29">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30">
-        <v>143</v>
-      </c>
-      <c r="E30">
-        <v>87</v>
-      </c>
-      <c r="F30">
-        <v>999</v>
-      </c>
-      <c r="G30">
-        <v>2052</v>
-      </c>
-      <c r="I30" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J30">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31">
-        <v>36</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>999</v>
-      </c>
-      <c r="G31">
-        <v>9999</v>
-      </c>
-      <c r="I31" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J31">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="30">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32">
-        <v>-20</v>
-      </c>
-      <c r="E32">
-        <v>-10</v>
-      </c>
-      <c r="F32">
-        <v>2003</v>
-      </c>
-      <c r="G32">
-        <v>2024</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I32" s="1">
-        <v>14.15</v>
-      </c>
-      <c r="J32">
-        <v>3.55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C33">
         <v>75</v>
       </c>
       <c r="D33">
-        <v>19</v>
+        <v>227760</v>
       </c>
       <c r="E33">
-        <v>26</v>
+        <v>999</v>
       </c>
       <c r="F33">
-        <v>999</v>
-      </c>
-      <c r="G33">
         <v>9999</v>
       </c>
-      <c r="I33" s="1">
+      <c r="H33" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J33">
+      <c r="I33">
         <v>3.63</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34">
         <v>25</v>
       </c>
       <c r="D34">
+        <v>70080</v>
+      </c>
+      <c r="E34">
+        <v>999</v>
+      </c>
+      <c r="F34">
+        <v>2027</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H34" s="1">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="I34">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30">
+      <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <v>87600</v>
+      </c>
+      <c r="E35">
+        <v>2012</v>
+      </c>
+      <c r="F35">
+        <v>9999</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36">
         <v>1</v>
       </c>
-      <c r="E34">
-        <v>8</v>
-      </c>
-      <c r="F34">
+      <c r="D36">
+        <v>17520</v>
+      </c>
+      <c r="E36">
         <v>999</v>
       </c>
-      <c r="G34">
-        <v>2027</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I34" s="1">
+      <c r="F36">
+        <v>9999</v>
+      </c>
+      <c r="H36" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J34">
+      <c r="I36">
         <v>3.63</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30">
-      <c r="A35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35">
-        <v>7</v>
-      </c>
-      <c r="E35">
-        <v>10</v>
-      </c>
-      <c r="F35">
-        <v>2012</v>
-      </c>
-      <c r="G35">
-        <v>9999</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36">
-        <v>999</v>
-      </c>
-      <c r="G36">
-        <v>9999</v>
-      </c>
-      <c r="I36" s="1">
-        <v>40.770000000000003</v>
-      </c>
-      <c r="J36">
-        <v>3.63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="30">
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C37">
+        <v>116</v>
+      </c>
       <c r="D37">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>2017</v>
       </c>
       <c r="F37">
-        <v>2017</v>
-      </c>
-      <c r="G37">
         <v>9999</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="G37" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C38">
+        <v>45</v>
+      </c>
       <c r="D38">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="F38">
-        <v>999</v>
-      </c>
-      <c r="G38">
         <v>9999</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C39">
+        <v>100</v>
+      </c>
       <c r="D39">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>2014</v>
       </c>
       <c r="F39">
-        <v>2014</v>
-      </c>
-      <c r="G39">
         <v>2019</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="G39" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40">
         <v>9</v>
       </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>2010</v>
+      </c>
       <c r="F40">
-        <v>2010</v>
-      </c>
-      <c r="G40">
         <v>2030</v>
       </c>
-      <c r="I40" s="1">
+      <c r="H40" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J40">
+      <c r="I40">
         <v>3.63</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C41">
         <v>13</v>
       </c>
+      <c r="D41">
+        <v>17520</v>
+      </c>
       <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="I41" s="1">
+        <v>999</v>
+      </c>
+      <c r="F41">
+        <v>9999</v>
+      </c>
+      <c r="H41" s="1">
         <v>18.350000000000001</v>
       </c>
-      <c r="J41">
+      <c r="I41">
         <v>2.87</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42">
         <v>10</v>
       </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>2014</v>
+      </c>
       <c r="F42">
-        <v>2014</v>
-      </c>
-      <c r="G42">
         <v>2035</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I42" s="1">
+      <c r="G42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H42" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J42">
+      <c r="I42">
         <v>3.63</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C43">
         <v>10</v>
       </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>2014</v>
+      </c>
       <c r="F43">
-        <v>2014</v>
-      </c>
-      <c r="G43">
         <v>2035</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I43" s="1">
+      <c r="G43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="J43">
+      <c r="I43">
         <v>3.63</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C44">
         <v>5</v>
       </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>2014</v>
+      </c>
       <c r="F44">
-        <v>2014</v>
-      </c>
-      <c r="G44">
         <v>2035</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I44" s="1">
+      <c r="G44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44" s="1">
         <v>18.350000000000001</v>
       </c>
-      <c r="J44">
+      <c r="I44">
         <v>2.87</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C45">
         <v>5</v>
       </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>2014</v>
+      </c>
       <c r="F45">
-        <v>2014</v>
-      </c>
-      <c r="G45">
         <v>2035</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I45" s="1">
+      <c r="G45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H45" s="1">
         <v>18.350000000000001</v>
       </c>
-      <c r="J45">
+      <c r="I45">
         <v>2.87</v>
       </c>
     </row>
@@ -2251,12 +2380,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B2">
         <v>43.22</v>
@@ -2267,7 +2396,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>49.27</v>
@@ -2278,7 +2407,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B4">
         <v>35.159999999999997</v>
@@ -2289,7 +2418,7 @@
     </row>
     <row r="6" spans="1:3" ht="45">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <v>30.83</v>

</xml_diff>

<commit_message>
began supply curves work, did not finish.
</commit_message>
<xml_diff>
--- a/inputs/PGE_Resources.xlsx
+++ b/inputs/PGE_Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4380" yWindow="0" windowWidth="23460" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>In-service date</t>
   </si>
@@ -284,6 +284,15 @@
   </si>
   <si>
     <t>STUPID</t>
+  </si>
+  <si>
+    <t>Overnight Capital Cost ($/kW)</t>
+  </si>
+  <si>
+    <t>Economic Life (Years)</t>
+  </si>
+  <si>
+    <t>WACC (%)</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1112,10 +1121,13 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" customWidth="1"/>
     <col min="7" max="7" width="43.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="65" customHeight="1">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="65" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -1138,16 +1150,25 @@
         <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1166,8 +1187,11 @@
       <c r="F2">
         <v>2015</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="H2" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1190,13 +1214,22 @@
         <v>76</v>
       </c>
       <c r="H3" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>67</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2650</v>
+      </c>
+      <c r="K3" s="1">
         <v>14.15</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>3.55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:13" ht="30">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1215,8 +1248,11 @@
       <c r="F4">
         <v>2014</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="H4" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1238,8 +1274,11 @@
       <c r="G5" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="30">
+      <c r="H5" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1261,8 +1300,11 @@
       <c r="G6" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="30">
+      <c r="H6" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1284,8 +1326,11 @@
       <c r="G7" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="30">
+      <c r="H7" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1307,8 +1352,11 @@
       <c r="G8" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="H8" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1331,16 +1379,25 @@
         <v>73</v>
       </c>
       <c r="H9" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>40</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2946</v>
+      </c>
+      <c r="K9" s="1">
         <v>23.44</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>3.78</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>9911</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1363,16 +1420,25 @@
         <v>74</v>
       </c>
       <c r="H10" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>40</v>
+      </c>
+      <c r="J10" s="1">
+        <v>2946</v>
+      </c>
+      <c r="K10" s="1">
         <v>23.44</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>3.78</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>11950</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1395,16 +1461,25 @@
         <v>45</v>
       </c>
       <c r="H11" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>35</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1121</v>
+      </c>
+      <c r="K11" s="1">
         <v>10.28</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>3.23</v>
       </c>
-      <c r="J11">
+      <c r="M11">
         <v>9260</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1424,16 +1499,25 @@
         <v>9999</v>
       </c>
       <c r="H12" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>35</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1121</v>
+      </c>
+      <c r="K12" s="1">
         <v>10.28</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>3.23</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>9260</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1453,16 +1537,25 @@
         <v>9999</v>
       </c>
       <c r="H13" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>35</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1121</v>
+      </c>
+      <c r="K13" s="1">
         <v>10.28</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>3.23</v>
       </c>
-      <c r="J13">
+      <c r="M13">
         <v>9260</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1482,16 +1575,25 @@
         <v>9999</v>
       </c>
       <c r="H14" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>35</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1121</v>
+      </c>
+      <c r="K14" s="1">
         <v>10.28</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>3.23</v>
       </c>
-      <c r="J14">
+      <c r="M14">
         <v>6800</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1514,16 +1616,25 @@
         <v>44</v>
       </c>
       <c r="H15" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>35</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1121</v>
+      </c>
+      <c r="K15" s="1">
         <v>10.28</v>
       </c>
-      <c r="I15">
+      <c r="L15">
         <v>3.23</v>
       </c>
-      <c r="J15">
+      <c r="M15">
         <v>6800</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1546,16 +1657,25 @@
         <v>46</v>
       </c>
       <c r="H16" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>35</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1121</v>
+      </c>
+      <c r="K16" s="1">
         <v>10.28</v>
       </c>
-      <c r="I16">
+      <c r="L16">
         <v>3.23</v>
       </c>
-      <c r="J16">
+      <c r="M16">
         <v>7100</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1575,16 +1695,25 @@
         <v>9999</v>
       </c>
       <c r="H17" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>35</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1121</v>
+      </c>
+      <c r="K17" s="1">
         <v>10.28</v>
       </c>
-      <c r="I17">
+      <c r="L17">
         <v>3.23</v>
       </c>
-      <c r="J17">
+      <c r="M17">
         <v>7043</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1608,13 +1737,22 @@
         <v>47</v>
       </c>
       <c r="H18" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <v>27</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K18" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>3.63</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1638,13 +1776,22 @@
         <v>48</v>
       </c>
       <c r="H19" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>27</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K19" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I19">
+      <c r="L19">
         <v>3.63</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1665,13 +1812,22 @@
         <v>9999</v>
       </c>
       <c r="H20" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>27</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K20" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I20">
+      <c r="L20">
         <v>3.63</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1691,13 +1847,22 @@
         <v>9999</v>
       </c>
       <c r="H21" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I21" s="1">
+        <v>27</v>
+      </c>
+      <c r="J21" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K21" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I21">
+      <c r="L21">
         <v>3.63</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1720,13 +1885,22 @@
         <v>51</v>
       </c>
       <c r="H22" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I22" s="1">
+        <v>67</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K22" s="1">
         <v>14.15</v>
       </c>
-      <c r="I22">
+      <c r="L22">
         <v>3.55</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1749,13 +1923,22 @@
         <v>51</v>
       </c>
       <c r="H23" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>67</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K23" s="1">
         <v>14.15</v>
       </c>
-      <c r="I23">
+      <c r="L23">
         <v>3.55</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1778,13 +1961,22 @@
         <v>51</v>
       </c>
       <c r="H24" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>67</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K24" s="1">
         <v>14.15</v>
       </c>
-      <c r="I24">
+      <c r="L24">
         <v>3.55</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1807,13 +1999,22 @@
         <v>51</v>
       </c>
       <c r="H25" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I25" s="1">
+        <v>67</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K25" s="1">
         <v>14.15</v>
       </c>
-      <c r="I25">
+      <c r="L25">
         <v>3.55</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1836,13 +2037,22 @@
         <v>50</v>
       </c>
       <c r="H26" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>67</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K26" s="1">
         <v>14.15</v>
       </c>
-      <c r="I26">
+      <c r="L26">
         <v>3.55</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1866,13 +2076,22 @@
         <v>49</v>
       </c>
       <c r="H27" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>67</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K27" s="1">
         <v>14.15</v>
       </c>
-      <c r="I27">
+      <c r="L27">
         <v>3.55</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1895,13 +2114,22 @@
         <v>49</v>
       </c>
       <c r="H28" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>67</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K28" s="1">
         <v>14.15</v>
       </c>
-      <c r="I28">
+      <c r="L28">
         <v>3.55</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1924,13 +2152,22 @@
         <v>49</v>
       </c>
       <c r="H29" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I29" s="1">
+        <v>67</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K29" s="1">
         <v>14.15</v>
       </c>
-      <c r="I29">
+      <c r="L29">
         <v>3.55</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1953,17 +2190,26 @@
         <v>53</v>
       </c>
       <c r="H30" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>67</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K30" s="1">
         <v>14.15</v>
       </c>
-      <c r="I30">
+      <c r="L30">
         <v>3.55</v>
       </c>
-      <c r="J30">
+      <c r="M30">
         <f>SUM(D28:D29)/8760</f>
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1984,13 +2230,22 @@
         <v>2052</v>
       </c>
       <c r="H31" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>67</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K31" s="1">
         <v>14.15</v>
       </c>
-      <c r="I31">
+      <c r="L31">
         <v>3.55</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -2010,13 +2265,22 @@
         <v>9999</v>
       </c>
       <c r="H32" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>67</v>
+      </c>
+      <c r="J32" s="1">
+        <v>1650</v>
+      </c>
+      <c r="K32" s="1">
         <v>14.15</v>
       </c>
-      <c r="I32">
+      <c r="L32">
         <v>3.55</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2036,13 +2300,22 @@
         <v>9999</v>
       </c>
       <c r="H33" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>27</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K33" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I33">
+      <c r="L33">
         <v>3.63</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -2065,13 +2338,22 @@
         <v>52</v>
       </c>
       <c r="H34" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I34" s="1">
+        <v>27</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K34" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I34">
+      <c r="L34">
         <v>3.63</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="30">
+    <row r="35" spans="1:12" ht="30">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -2093,8 +2375,11 @@
       <c r="G35" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="H35" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -2114,13 +2399,22 @@
         <v>9999</v>
       </c>
       <c r="H36" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>27</v>
+      </c>
+      <c r="J36" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K36" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I36">
+      <c r="L36">
         <v>3.63</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30">
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -2142,8 +2436,11 @@
       <c r="G37" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="H37" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -2162,8 +2459,11 @@
       <c r="F38">
         <v>9999</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="H38" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -2185,8 +2485,11 @@
       <c r="G39" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="H39" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>56</v>
       </c>
@@ -2206,13 +2509,22 @@
         <v>2030</v>
       </c>
       <c r="H40" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I40" s="1">
+        <v>27</v>
+      </c>
+      <c r="J40" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K40" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I40">
+      <c r="L40">
         <v>3.63</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>58</v>
       </c>
@@ -2232,13 +2544,22 @@
         <v>9999</v>
       </c>
       <c r="H41" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>25</v>
+      </c>
+      <c r="J41" s="1">
+        <v>2797</v>
+      </c>
+      <c r="K41" s="1">
         <v>18.350000000000001</v>
       </c>
-      <c r="I41">
+      <c r="L41">
         <v>2.87</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -2261,13 +2582,22 @@
         <v>65</v>
       </c>
       <c r="H42" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I42" s="1">
+        <v>27</v>
+      </c>
+      <c r="J42" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K42" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I42">
+      <c r="L42">
         <v>3.63</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -2290,13 +2620,22 @@
         <v>65</v>
       </c>
       <c r="H43" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>27</v>
+      </c>
+      <c r="J43" s="1">
+        <v>2213</v>
+      </c>
+      <c r="K43" s="1">
         <v>40.770000000000003</v>
       </c>
-      <c r="I43">
+      <c r="L43">
         <v>3.63</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -2319,13 +2658,22 @@
         <v>65</v>
       </c>
       <c r="H44" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I44" s="1">
+        <v>25</v>
+      </c>
+      <c r="J44" s="1">
+        <v>2797</v>
+      </c>
+      <c r="K44" s="1">
         <v>18.350000000000001</v>
       </c>
-      <c r="I44">
+      <c r="L44">
         <v>2.87</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>68</v>
       </c>
@@ -2348,9 +2696,18 @@
         <v>65</v>
       </c>
       <c r="H45" s="1">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="I45" s="1">
+        <v>25</v>
+      </c>
+      <c r="J45" s="1">
+        <v>2797</v>
+      </c>
+      <c r="K45" s="1">
         <v>18.350000000000001</v>
       </c>
-      <c r="I45">
+      <c r="L45">
         <v>2.87</v>
       </c>
     </row>

</xml_diff>